<commit_message>
Added operating emissions to heat exchanger network model
</commit_message>
<xml_diff>
--- a/data/JonesP3.xlsx
+++ b/data/JonesP3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="EAM" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="69">
   <si>
     <t>HEX</t>
   </si>
@@ -229,6 +229,9 @@
   </si>
   <si>
     <t>HU</t>
+  </si>
+  <si>
+    <t>tonsCO2emissionsperkWh</t>
   </si>
 </sst>
 </file>
@@ -1779,9 +1782,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
+      <selection pane="bottomLeft" activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1833,6 +1836,9 @@
       <c r="N1" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="O1" s="1" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -2051,8 +2057,7 @@
         <v>0.08</v>
       </c>
       <c r="O6" s="4">
-        <f>K6*J6</f>
-        <v>15857600</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="7" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2100,8 +2105,7 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="O7" s="1">
-        <f>K7*J7</f>
-        <v>39177600</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -2325,8 +2329,7 @@
         <v>0.08</v>
       </c>
       <c r="O12" s="4">
-        <f>K12*(J12-I12)</f>
-        <v>6004800</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="13" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2374,8 +2377,7 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="O13" s="1">
-        <f>K13*(J13-I13)</f>
-        <v>29023200</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -2467,7 +2469,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
     </sheetView>

</xml_diff>

<commit_message>
Updated DE for Pareto optimization with a new twin function which removes similar solutions
</commit_message>
<xml_diff>
--- a/data/JonesP3.xlsx
+++ b/data/JonesP3.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF56A49A-7AE4-4E44-ACE2-A075AF097662}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D718D461-191A-4905-9511-EF4E0E245903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23280" yWindow="3945" windowWidth="21600" windowHeight="12735" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EAM" sheetId="1" r:id="rId1"/>
@@ -235,7 +235,7 @@
     <t>tonsCO2emissionsperkWh</t>
   </si>
   <si>
-    <t>TACEmissionWeightFactor</t>
+    <t>AbsHeatLoadTol</t>
   </si>
 </sst>
 </file>
@@ -2484,14 +2484,15 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J13" sqref="J13"/>
+      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2519,7 +2520,7 @@
         <v>10</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>